<commit_message>
update: -added db save option -added test project
</commit_message>
<xml_diff>
--- a/TestPathwayMaker/TestExcelFiles/OurimbahMNGT30072018S1TESTFILE.xlsx
+++ b/TestPathwayMaker/TestExcelFiles/OurimbahMNGT30072018S1TESTFILE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh462\Documents\DEV\CoursePathwayMaker\TestPathwayMaker\TestExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CoursePathwayMaker\TestPathwayMaker\TestExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D387A21C-892C-481D-BDE0-75E0423A334F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ourimbah" sheetId="1" r:id="rId1"/>
@@ -26,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
-    <t>Students</t>
-  </si>
-  <si>
     <t xml:space="preserve">MNGT3002 </t>
   </si>
   <si>
@@ -116,11 +114,14 @@
   <si>
     <t>MNGT2006</t>
   </si>
+  <si>
+    <t>Students</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,11 +445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +477,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -502,13 +503,13 @@
         <v>3232703</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -519,14 +520,14 @@
         <v>3038097</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -537,16 +538,16 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -555,22 +556,22 @@
         <v>3236903</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,13 +580,13 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -595,20 +596,20 @@
         <v>3207863</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -618,7 +619,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -631,7 +632,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -642,11 +643,11 @@
         <v>3260469</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>

</xml_diff>